<commit_message>
Paint, Racks and Flex expenditures
</commit_message>
<xml_diff>
--- a/Financial Accounts/Expenditure Inccured on office.xlsx
+++ b/Financial Accounts/Expenditure Inccured on office.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="86">
   <si>
     <t>Sultan</t>
   </si>
@@ -236,13 +236,76 @@
   </si>
   <si>
     <t>Investment\Widrawls</t>
+  </si>
+  <si>
+    <t>Phase III</t>
+  </si>
+  <si>
+    <t>Moni</t>
+  </si>
+  <si>
+    <t>Widrawl + returns</t>
+  </si>
+  <si>
+    <t>Paint</t>
+  </si>
+  <si>
+    <t>Wood material</t>
+  </si>
+  <si>
+    <t>Keelen</t>
+  </si>
+  <si>
+    <t>Lock (sultan)</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Paint operations</t>
+  </si>
+  <si>
+    <t>Total cost</t>
+  </si>
+  <si>
+    <t>Remaining amount</t>
+  </si>
+  <si>
+    <t>labour</t>
+  </si>
+  <si>
+    <t>paint material</t>
+  </si>
+  <si>
+    <t>seeri</t>
+  </si>
+  <si>
+    <t>flex</t>
+  </si>
+  <si>
+    <t>Donkey cart</t>
+  </si>
+  <si>
+    <t>Carpenter</t>
+  </si>
+  <si>
+    <t>Zink</t>
+  </si>
+  <si>
+    <t>grey teen paint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">labour </t>
+  </si>
+  <si>
+    <t>inouguration+Van Rent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,6 +349,19 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -307,13 +383,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,11 +694,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K95"/>
+  <dimension ref="A1:K126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A107" sqref="A107"/>
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1508,6 +1587,210 @@
       <c r="I95" s="1">
         <f>E95+G95</f>
         <v>54936</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B98" s="7"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C99" s="7">
+        <v>20630</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C100" s="7">
+        <v>7900</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C101" s="7">
+        <v>3375</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C102" s="7">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C103" s="7">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C104" s="7">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C105" s="7">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C106" s="7">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C107" s="7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C108" s="6">
+        <f>SUM(C100:C107)</f>
+        <v>20210</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C109" s="7">
+        <f>C99-C108</f>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B113" s="7"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C114" s="7">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C115" s="7">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C116" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C117" s="7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C118" s="7">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C119" s="7">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C120" s="7">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C121" s="7">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C122" s="7">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C123" s="7">
+        <v>5200</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="7"/>
+      <c r="C124" s="7"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="7"/>
+      <c r="C125" s="7"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C126" s="6">
+        <f>SUM(C114:C125)</f>
+        <v>12750</v>
       </c>
     </row>
   </sheetData>

</xml_diff>